<commit_message>
Doc: Added actual hours
</commit_message>
<xml_diff>
--- a/Release Planning/Release5_ planning.xlsx
+++ b/Release Planning/Release5_ planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C8CA4A-54A6-4ECD-B381-642DD25293E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AB16D9-6017-4837-820C-F49F9817E51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,10 +103,6 @@
     <t>Total Tasks</t>
   </si>
   <si>
-    <t>Release 6
-Planning</t>
-  </si>
-  <si>
     <t>Test Case
 Execution</t>
   </si>
@@ -159,12 +155,15 @@
   <si>
     <t>Abdallah</t>
   </si>
+  <si>
+    <t>Bug Fixes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -216,12 +215,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -342,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -440,15 +433,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -527,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,89 +550,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -657,48 +597,56 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,20 +866,20 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F978"/>
+  <dimension ref="A1:F972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40" style="58" customWidth="1"/>
+    <col min="3" max="3" width="40" style="37" customWidth="1"/>
     <col min="4" max="4" width="31.140625" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32" style="68" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -941,7 +889,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -955,14 +903,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>24</v>
+      <c r="A2" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>30</v>
       </c>
       <c r="D2" s="5">
         <v>2</v>
@@ -970,17 +918,17 @@
       <c r="E2" s="23">
         <v>2</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>29</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
@@ -988,17 +936,17 @@
       <c r="E3" s="23">
         <v>2</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="5">
         <v>2</v>
@@ -1006,17 +954,17 @@
       <c r="E4" s="23">
         <v>2</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>29</v>
       </c>
       <c r="D5" s="5">
         <v>2</v>
@@ -1024,22 +972,22 @@
       <c r="E5" s="23">
         <v>2</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="51"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="5"/>
       <c r="E6" s="23"/>
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="51"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="5"/>
       <c r="E7" s="23"/>
       <c r="F7" s="26"/>
@@ -1047,3099 +995,3066 @@
     <row r="8" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="52"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="8"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="62"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C10" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="26" t="s">
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <v>4</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3</v>
+      </c>
+      <c r="E13" s="27">
+        <v>2</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="23">
+        <v>5</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="20">
+        <f>COUNTIF(F2:F15,"Doing")+COUNTIF(F2:F15,"Done")+COUNTIF(F2:F15,"To do")</f>
+        <v>10</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="17">
+        <f>COUNTIF(F2:F15,"Doing")</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="39">
+        <f>(D17/D16)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="54">
+        <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="35" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="63"/>
-    </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="63"/>
-    </row>
-    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="62"/>
-    </row>
-    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="43">
-        <v>3</v>
-      </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="64" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="64"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="64"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="64"/>
+      <c r="D18" s="18">
+        <f>COUNTIF(F2:F15,"To do")</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="39">
+        <f>D18/D16</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="54"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="19">
+        <f>COUNTIF(F2:F15,"Done")</f>
+        <v>10</v>
+      </c>
+      <c r="E19" s="39">
+        <f>D19/D16</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="54"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="20">
-        <f>COUNTIF(F2:F20,"Doing")+COUNTIF(F2:F20,"Done")+COUNTIF(F2:F20,"To do")</f>
-        <v>10</v>
-      </c>
-      <c r="E22" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="65" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="17">
-        <f>COUNTIF(F2:F20,"Doing")</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="60">
-        <f>(D23/D22)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="66">
-        <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="18">
-        <f>COUNTIF(F2:F20,"To do")</f>
-        <v>6</v>
-      </c>
-      <c r="E24" s="60">
-        <f>D24/D22</f>
-        <v>0.6</v>
-      </c>
-      <c r="F24" s="66"/>
-    </row>
-    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="19">
-        <f>COUNTIF(F2:F20,"Done")</f>
-        <v>4</v>
-      </c>
-      <c r="E25" s="60">
-        <f>D25/D22</f>
-        <v>0.4</v>
-      </c>
-      <c r="F25" s="66"/>
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F23" s="43"/>
+    </row>
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F25" s="43"/>
+    </row>
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F27" s="67"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F28" s="67"/>
+      <c r="F28" s="43"/>
     </row>
     <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F29" s="67"/>
+      <c r="F29" s="43"/>
     </row>
     <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F30" s="67"/>
+      <c r="F30" s="43"/>
     </row>
     <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F31" s="67"/>
+      <c r="F31" s="43"/>
     </row>
     <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F32" s="67"/>
+      <c r="F32" s="43"/>
     </row>
     <row r="33" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F33" s="67"/>
+      <c r="F33" s="43"/>
     </row>
     <row r="34" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F34" s="67"/>
+      <c r="F34" s="43"/>
     </row>
     <row r="35" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F35" s="67"/>
+      <c r="F35" s="43"/>
     </row>
     <row r="36" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F36" s="67"/>
+      <c r="F36" s="43"/>
     </row>
     <row r="37" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F37" s="67"/>
+      <c r="F37" s="43"/>
     </row>
     <row r="38" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F38" s="67"/>
+      <c r="F38" s="43"/>
     </row>
     <row r="39" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F39" s="67"/>
+      <c r="F39" s="43"/>
     </row>
     <row r="40" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F40" s="67"/>
+      <c r="F40" s="43"/>
     </row>
     <row r="41" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F41" s="67"/>
+      <c r="F41" s="43"/>
     </row>
     <row r="42" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F42" s="67"/>
+      <c r="F42" s="43"/>
     </row>
     <row r="43" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F43" s="67"/>
+      <c r="F43" s="43"/>
     </row>
     <row r="44" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F44" s="67"/>
+      <c r="F44" s="43"/>
     </row>
     <row r="45" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F45" s="67"/>
+      <c r="F45" s="43"/>
     </row>
     <row r="46" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F46" s="67"/>
+      <c r="F46" s="43"/>
     </row>
     <row r="47" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F47" s="67"/>
+      <c r="F47" s="43"/>
     </row>
     <row r="48" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F48" s="67"/>
+      <c r="F48" s="43"/>
     </row>
     <row r="49" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F49" s="67"/>
+      <c r="F49" s="43"/>
     </row>
     <row r="50" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F50" s="67"/>
+      <c r="F50" s="43"/>
     </row>
     <row r="51" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F51" s="67"/>
+      <c r="F51" s="43"/>
     </row>
     <row r="52" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F52" s="67"/>
+      <c r="F52" s="43"/>
     </row>
     <row r="53" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F53" s="67"/>
+      <c r="F53" s="43"/>
     </row>
     <row r="54" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F54" s="67"/>
+      <c r="F54" s="43"/>
     </row>
     <row r="55" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F55" s="67"/>
+      <c r="F55" s="43"/>
     </row>
     <row r="56" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F56" s="67"/>
+      <c r="F56" s="43"/>
     </row>
     <row r="57" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F57" s="67"/>
+      <c r="F57" s="43"/>
     </row>
     <row r="58" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F58" s="67"/>
+      <c r="F58" s="43"/>
     </row>
     <row r="59" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F59" s="67"/>
+      <c r="F59" s="43"/>
     </row>
     <row r="60" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F60" s="67"/>
+      <c r="F60" s="43"/>
     </row>
     <row r="61" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F61" s="67"/>
+      <c r="F61" s="43"/>
     </row>
     <row r="62" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F62" s="67"/>
+      <c r="F62" s="43"/>
     </row>
     <row r="63" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F63" s="67"/>
+      <c r="F63" s="43"/>
     </row>
     <row r="64" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F64" s="67"/>
+      <c r="F64" s="43"/>
     </row>
     <row r="65" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F65" s="67"/>
+      <c r="F65" s="43"/>
     </row>
     <row r="66" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F66" s="67"/>
+      <c r="F66" s="43"/>
     </row>
     <row r="67" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F67" s="67"/>
+      <c r="F67" s="43"/>
     </row>
     <row r="68" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F68" s="67"/>
+      <c r="F68" s="43"/>
     </row>
     <row r="69" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F69" s="67"/>
+      <c r="F69" s="43"/>
     </row>
     <row r="70" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F70" s="67"/>
+      <c r="F70" s="43"/>
     </row>
     <row r="71" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F71" s="67"/>
+      <c r="F71" s="43"/>
     </row>
     <row r="72" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F72" s="67"/>
+      <c r="F72" s="43"/>
     </row>
     <row r="73" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F73" s="67"/>
+      <c r="F73" s="43"/>
     </row>
     <row r="74" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F74" s="67"/>
+      <c r="F74" s="43"/>
     </row>
     <row r="75" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F75" s="67"/>
+      <c r="F75" s="43"/>
     </row>
     <row r="76" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F76" s="67"/>
+      <c r="F76" s="43"/>
     </row>
     <row r="77" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F77" s="67"/>
+      <c r="F77" s="43"/>
     </row>
     <row r="78" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F78" s="67"/>
+      <c r="F78" s="43"/>
     </row>
     <row r="79" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F79" s="67"/>
+      <c r="F79" s="43"/>
     </row>
     <row r="80" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F80" s="67"/>
+      <c r="F80" s="43"/>
     </row>
     <row r="81" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F81" s="67"/>
+      <c r="F81" s="43"/>
     </row>
     <row r="82" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F82" s="67"/>
+      <c r="F82" s="43"/>
     </row>
     <row r="83" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F83" s="67"/>
+      <c r="F83" s="43"/>
     </row>
     <row r="84" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F84" s="67"/>
+      <c r="F84" s="43"/>
     </row>
     <row r="85" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F85" s="67"/>
+      <c r="F85" s="43"/>
     </row>
     <row r="86" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F86" s="67"/>
+      <c r="F86" s="43"/>
     </row>
     <row r="87" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F87" s="67"/>
+      <c r="F87" s="43"/>
     </row>
     <row r="88" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F88" s="67"/>
+      <c r="F88" s="43"/>
     </row>
     <row r="89" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F89" s="67"/>
+      <c r="F89" s="43"/>
     </row>
     <row r="90" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F90" s="67"/>
+      <c r="F90" s="43"/>
     </row>
     <row r="91" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F91" s="67"/>
+      <c r="F91" s="43"/>
     </row>
     <row r="92" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F92" s="67"/>
+      <c r="F92" s="43"/>
     </row>
     <row r="93" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F93" s="67"/>
+      <c r="F93" s="43"/>
     </row>
     <row r="94" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F94" s="67"/>
+      <c r="F94" s="43"/>
     </row>
     <row r="95" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F95" s="67"/>
+      <c r="F95" s="43"/>
     </row>
     <row r="96" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F96" s="67"/>
+      <c r="F96" s="43"/>
     </row>
     <row r="97" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F97" s="67"/>
+      <c r="F97" s="43"/>
     </row>
     <row r="98" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F98" s="67"/>
+      <c r="F98" s="43"/>
     </row>
     <row r="99" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F99" s="67"/>
+      <c r="F99" s="43"/>
     </row>
     <row r="100" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F100" s="67"/>
+      <c r="F100" s="43"/>
     </row>
     <row r="101" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F101" s="67"/>
+      <c r="F101" s="43"/>
     </row>
     <row r="102" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F102" s="67"/>
+      <c r="F102" s="43"/>
     </row>
     <row r="103" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F103" s="67"/>
+      <c r="F103" s="43"/>
     </row>
     <row r="104" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F104" s="67"/>
+      <c r="F104" s="43"/>
     </row>
     <row r="105" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F105" s="67"/>
+      <c r="F105" s="43"/>
     </row>
     <row r="106" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F106" s="67"/>
+      <c r="F106" s="43"/>
     </row>
     <row r="107" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F107" s="67"/>
+      <c r="F107" s="43"/>
     </row>
     <row r="108" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F108" s="67"/>
+      <c r="F108" s="43"/>
     </row>
     <row r="109" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F109" s="67"/>
+      <c r="F109" s="43"/>
     </row>
     <row r="110" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F110" s="67"/>
+      <c r="F110" s="43"/>
     </row>
     <row r="111" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F111" s="67"/>
+      <c r="F111" s="43"/>
     </row>
     <row r="112" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F112" s="67"/>
+      <c r="F112" s="43"/>
     </row>
     <row r="113" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F113" s="67"/>
+      <c r="F113" s="43"/>
     </row>
     <row r="114" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F114" s="67"/>
+      <c r="F114" s="43"/>
     </row>
     <row r="115" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F115" s="67"/>
+      <c r="F115" s="43"/>
     </row>
     <row r="116" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F116" s="67"/>
+      <c r="F116" s="43"/>
     </row>
     <row r="117" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F117" s="67"/>
+      <c r="F117" s="43"/>
     </row>
     <row r="118" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F118" s="67"/>
+      <c r="F118" s="43"/>
     </row>
     <row r="119" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F119" s="67"/>
+      <c r="F119" s="43"/>
     </row>
     <row r="120" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F120" s="67"/>
+      <c r="F120" s="43"/>
     </row>
     <row r="121" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F121" s="67"/>
+      <c r="F121" s="43"/>
     </row>
     <row r="122" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F122" s="67"/>
+      <c r="F122" s="43"/>
     </row>
     <row r="123" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F123" s="67"/>
+      <c r="F123" s="43"/>
     </row>
     <row r="124" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F124" s="67"/>
+      <c r="F124" s="43"/>
     </row>
     <row r="125" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F125" s="67"/>
+      <c r="F125" s="43"/>
     </row>
     <row r="126" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F126" s="67"/>
+      <c r="F126" s="43"/>
     </row>
     <row r="127" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F127" s="67"/>
+      <c r="F127" s="43"/>
     </row>
     <row r="128" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F128" s="67"/>
+      <c r="F128" s="43"/>
     </row>
     <row r="129" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F129" s="67"/>
+      <c r="F129" s="43"/>
     </row>
     <row r="130" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F130" s="67"/>
+      <c r="F130" s="43"/>
     </row>
     <row r="131" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F131" s="67"/>
+      <c r="F131" s="43"/>
     </row>
     <row r="132" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F132" s="67"/>
+      <c r="F132" s="43"/>
     </row>
     <row r="133" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F133" s="67"/>
+      <c r="F133" s="43"/>
     </row>
     <row r="134" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F134" s="67"/>
+      <c r="F134" s="43"/>
     </row>
     <row r="135" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F135" s="67"/>
+      <c r="F135" s="43"/>
     </row>
     <row r="136" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F136" s="67"/>
+      <c r="F136" s="43"/>
     </row>
     <row r="137" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F137" s="67"/>
+      <c r="F137" s="43"/>
     </row>
     <row r="138" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F138" s="67"/>
+      <c r="F138" s="43"/>
     </row>
     <row r="139" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F139" s="67"/>
+      <c r="F139" s="43"/>
     </row>
     <row r="140" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F140" s="67"/>
+      <c r="F140" s="43"/>
     </row>
     <row r="141" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F141" s="67"/>
+      <c r="F141" s="43"/>
     </row>
     <row r="142" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F142" s="67"/>
+      <c r="F142" s="43"/>
     </row>
     <row r="143" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F143" s="67"/>
+      <c r="F143" s="43"/>
     </row>
     <row r="144" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F144" s="67"/>
+      <c r="F144" s="43"/>
     </row>
     <row r="145" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F145" s="67"/>
+      <c r="F145" s="43"/>
     </row>
     <row r="146" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F146" s="67"/>
+      <c r="F146" s="43"/>
     </row>
     <row r="147" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F147" s="67"/>
+      <c r="F147" s="43"/>
     </row>
     <row r="148" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F148" s="67"/>
+      <c r="F148" s="43"/>
     </row>
     <row r="149" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F149" s="67"/>
+      <c r="F149" s="43"/>
     </row>
     <row r="150" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F150" s="67"/>
+      <c r="F150" s="43"/>
     </row>
     <row r="151" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F151" s="67"/>
+      <c r="F151" s="43"/>
     </row>
     <row r="152" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F152" s="67"/>
+      <c r="F152" s="43"/>
     </row>
     <row r="153" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F153" s="67"/>
+      <c r="F153" s="43"/>
     </row>
     <row r="154" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F154" s="67"/>
+      <c r="F154" s="43"/>
     </row>
     <row r="155" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F155" s="67"/>
+      <c r="F155" s="43"/>
     </row>
     <row r="156" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F156" s="67"/>
+      <c r="F156" s="43"/>
     </row>
     <row r="157" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F157" s="67"/>
+      <c r="F157" s="43"/>
     </row>
     <row r="158" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F158" s="67"/>
+      <c r="F158" s="43"/>
     </row>
     <row r="159" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F159" s="67"/>
+      <c r="F159" s="43"/>
     </row>
     <row r="160" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F160" s="67"/>
+      <c r="F160" s="43"/>
     </row>
     <row r="161" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F161" s="67"/>
+      <c r="F161" s="43"/>
     </row>
     <row r="162" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F162" s="67"/>
+      <c r="F162" s="43"/>
     </row>
     <row r="163" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F163" s="67"/>
+      <c r="F163" s="43"/>
     </row>
     <row r="164" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F164" s="67"/>
+      <c r="F164" s="43"/>
     </row>
     <row r="165" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F165" s="67"/>
+      <c r="F165" s="43"/>
     </row>
     <row r="166" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F166" s="67"/>
+      <c r="F166" s="43"/>
     </row>
     <row r="167" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F167" s="67"/>
+      <c r="F167" s="43"/>
     </row>
     <row r="168" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F168" s="67"/>
+      <c r="F168" s="43"/>
     </row>
     <row r="169" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F169" s="67"/>
+      <c r="F169" s="43"/>
     </row>
     <row r="170" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F170" s="67"/>
+      <c r="F170" s="43"/>
     </row>
     <row r="171" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F171" s="67"/>
+      <c r="F171" s="43"/>
     </row>
     <row r="172" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F172" s="67"/>
+      <c r="F172" s="43"/>
     </row>
     <row r="173" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F173" s="67"/>
+      <c r="F173" s="43"/>
     </row>
     <row r="174" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F174" s="67"/>
+      <c r="F174" s="43"/>
     </row>
     <row r="175" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F175" s="67"/>
+      <c r="F175" s="43"/>
     </row>
     <row r="176" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F176" s="67"/>
+      <c r="F176" s="43"/>
     </row>
     <row r="177" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F177" s="67"/>
+      <c r="F177" s="43"/>
     </row>
     <row r="178" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F178" s="67"/>
+      <c r="F178" s="43"/>
     </row>
     <row r="179" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F179" s="67"/>
+      <c r="F179" s="43"/>
     </row>
     <row r="180" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F180" s="67"/>
+      <c r="F180" s="43"/>
     </row>
     <row r="181" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F181" s="67"/>
+      <c r="F181" s="43"/>
     </row>
     <row r="182" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F182" s="67"/>
+      <c r="F182" s="43"/>
     </row>
     <row r="183" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F183" s="67"/>
+      <c r="F183" s="43"/>
     </row>
     <row r="184" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F184" s="67"/>
+      <c r="F184" s="43"/>
     </row>
     <row r="185" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F185" s="67"/>
+      <c r="F185" s="43"/>
     </row>
     <row r="186" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F186" s="67"/>
+      <c r="F186" s="43"/>
     </row>
     <row r="187" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F187" s="67"/>
+      <c r="F187" s="43"/>
     </row>
     <row r="188" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F188" s="67"/>
+      <c r="F188" s="43"/>
     </row>
     <row r="189" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F189" s="67"/>
+      <c r="F189" s="43"/>
     </row>
     <row r="190" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F190" s="67"/>
+      <c r="F190" s="43"/>
     </row>
     <row r="191" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F191" s="67"/>
+      <c r="F191" s="43"/>
     </row>
     <row r="192" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F192" s="67"/>
+      <c r="F192" s="43"/>
     </row>
     <row r="193" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F193" s="67"/>
+      <c r="F193" s="43"/>
     </row>
     <row r="194" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F194" s="67"/>
+      <c r="F194" s="43"/>
     </row>
     <row r="195" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F195" s="67"/>
+      <c r="F195" s="43"/>
     </row>
     <row r="196" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F196" s="67"/>
+      <c r="F196" s="43"/>
     </row>
     <row r="197" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F197" s="67"/>
+      <c r="F197" s="43"/>
     </row>
     <row r="198" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F198" s="67"/>
+      <c r="F198" s="43"/>
     </row>
     <row r="199" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F199" s="67"/>
+      <c r="F199" s="43"/>
     </row>
     <row r="200" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F200" s="67"/>
+      <c r="F200" s="43"/>
     </row>
     <row r="201" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F201" s="67"/>
+      <c r="F201" s="43"/>
     </row>
     <row r="202" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F202" s="67"/>
+      <c r="F202" s="43"/>
     </row>
     <row r="203" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F203" s="67"/>
+      <c r="F203" s="43"/>
     </row>
     <row r="204" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F204" s="67"/>
+      <c r="F204" s="43"/>
     </row>
     <row r="205" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F205" s="67"/>
+      <c r="F205" s="43"/>
     </row>
     <row r="206" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F206" s="67"/>
+      <c r="F206" s="43"/>
     </row>
     <row r="207" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F207" s="67"/>
+      <c r="F207" s="43"/>
     </row>
     <row r="208" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F208" s="67"/>
+      <c r="F208" s="43"/>
     </row>
     <row r="209" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F209" s="67"/>
+      <c r="F209" s="43"/>
     </row>
     <row r="210" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F210" s="67"/>
+      <c r="F210" s="43"/>
     </row>
     <row r="211" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F211" s="67"/>
+      <c r="F211" s="43"/>
     </row>
     <row r="212" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F212" s="67"/>
+      <c r="F212" s="43"/>
     </row>
     <row r="213" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F213" s="67"/>
+      <c r="F213" s="43"/>
     </row>
     <row r="214" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F214" s="67"/>
+      <c r="F214" s="43"/>
     </row>
     <row r="215" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F215" s="67"/>
+      <c r="F215" s="43"/>
     </row>
     <row r="216" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F216" s="67"/>
+      <c r="F216" s="43"/>
     </row>
     <row r="217" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F217" s="67"/>
+      <c r="F217" s="43"/>
     </row>
     <row r="218" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F218" s="67"/>
+      <c r="F218" s="43"/>
     </row>
     <row r="219" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F219" s="67"/>
+      <c r="F219" s="43"/>
     </row>
     <row r="220" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F220" s="67"/>
+      <c r="F220" s="43"/>
     </row>
     <row r="221" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F221" s="67"/>
+      <c r="F221" s="43"/>
     </row>
     <row r="222" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F222" s="67"/>
+      <c r="F222" s="43"/>
     </row>
     <row r="223" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F223" s="67"/>
+      <c r="F223" s="43"/>
     </row>
     <row r="224" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F224" s="67"/>
+      <c r="F224" s="43"/>
     </row>
     <row r="225" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F225" s="67"/>
+      <c r="F225" s="43"/>
     </row>
     <row r="226" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F226" s="67"/>
+      <c r="F226" s="43"/>
     </row>
     <row r="227" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F227" s="67"/>
+      <c r="F227" s="43"/>
     </row>
     <row r="228" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F228" s="67"/>
+      <c r="F228" s="43"/>
     </row>
     <row r="229" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F229" s="67"/>
+      <c r="F229" s="43"/>
     </row>
     <row r="230" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F230" s="67"/>
+      <c r="F230" s="43"/>
     </row>
     <row r="231" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F231" s="67"/>
+      <c r="F231" s="43"/>
     </row>
     <row r="232" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F232" s="67"/>
+      <c r="F232" s="43"/>
     </row>
     <row r="233" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F233" s="67"/>
+      <c r="F233" s="43"/>
     </row>
     <row r="234" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F234" s="67"/>
+      <c r="F234" s="43"/>
     </row>
     <row r="235" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F235" s="67"/>
+      <c r="F235" s="43"/>
     </row>
     <row r="236" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F236" s="67"/>
+      <c r="F236" s="43"/>
     </row>
     <row r="237" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F237" s="67"/>
+      <c r="F237" s="43"/>
     </row>
     <row r="238" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F238" s="67"/>
+      <c r="F238" s="43"/>
     </row>
     <row r="239" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F239" s="67"/>
+      <c r="F239" s="43"/>
     </row>
     <row r="240" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F240" s="67"/>
+      <c r="F240" s="43"/>
     </row>
     <row r="241" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F241" s="67"/>
+      <c r="F241" s="43"/>
     </row>
     <row r="242" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F242" s="67"/>
+      <c r="F242" s="43"/>
     </row>
     <row r="243" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F243" s="67"/>
+      <c r="F243" s="43"/>
     </row>
     <row r="244" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F244" s="67"/>
+      <c r="F244" s="43"/>
     </row>
     <row r="245" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F245" s="67"/>
+      <c r="F245" s="43"/>
     </row>
     <row r="246" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F246" s="67"/>
+      <c r="F246" s="43"/>
     </row>
     <row r="247" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F247" s="67"/>
+      <c r="F247" s="43"/>
     </row>
     <row r="248" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F248" s="67"/>
+      <c r="F248" s="43"/>
     </row>
     <row r="249" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F249" s="67"/>
+      <c r="F249" s="43"/>
     </row>
     <row r="250" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F250" s="67"/>
+      <c r="F250" s="43"/>
     </row>
     <row r="251" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F251" s="67"/>
+      <c r="F251" s="43"/>
     </row>
     <row r="252" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F252" s="67"/>
+      <c r="F252" s="43"/>
     </row>
     <row r="253" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F253" s="67"/>
+      <c r="F253" s="43"/>
     </row>
     <row r="254" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F254" s="67"/>
+      <c r="F254" s="43"/>
     </row>
     <row r="255" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F255" s="67"/>
+      <c r="F255" s="43"/>
     </row>
     <row r="256" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F256" s="67"/>
+      <c r="F256" s="43"/>
     </row>
     <row r="257" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F257" s="67"/>
+      <c r="F257" s="43"/>
     </row>
     <row r="258" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F258" s="67"/>
+      <c r="F258" s="43"/>
     </row>
     <row r="259" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F259" s="67"/>
+      <c r="F259" s="43"/>
     </row>
     <row r="260" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F260" s="67"/>
+      <c r="F260" s="43"/>
     </row>
     <row r="261" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F261" s="67"/>
+      <c r="F261" s="43"/>
     </row>
     <row r="262" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F262" s="67"/>
+      <c r="F262" s="43"/>
     </row>
     <row r="263" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F263" s="67"/>
+      <c r="F263" s="43"/>
     </row>
     <row r="264" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F264" s="67"/>
+      <c r="F264" s="43"/>
     </row>
     <row r="265" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F265" s="67"/>
+      <c r="F265" s="43"/>
     </row>
     <row r="266" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F266" s="67"/>
+      <c r="F266" s="43"/>
     </row>
     <row r="267" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F267" s="67"/>
+      <c r="F267" s="43"/>
     </row>
     <row r="268" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F268" s="67"/>
+      <c r="F268" s="43"/>
     </row>
     <row r="269" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F269" s="67"/>
+      <c r="F269" s="43"/>
     </row>
     <row r="270" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F270" s="67"/>
+      <c r="F270" s="43"/>
     </row>
     <row r="271" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F271" s="67"/>
+      <c r="F271" s="43"/>
     </row>
     <row r="272" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F272" s="67"/>
+      <c r="F272" s="43"/>
     </row>
     <row r="273" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F273" s="67"/>
+      <c r="F273" s="43"/>
     </row>
     <row r="274" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F274" s="67"/>
+      <c r="F274" s="43"/>
     </row>
     <row r="275" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F275" s="67"/>
+      <c r="F275" s="43"/>
     </row>
     <row r="276" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F276" s="67"/>
+      <c r="F276" s="43"/>
     </row>
     <row r="277" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F277" s="67"/>
+      <c r="F277" s="43"/>
     </row>
     <row r="278" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F278" s="67"/>
+      <c r="F278" s="43"/>
     </row>
     <row r="279" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F279" s="67"/>
+      <c r="F279" s="43"/>
     </row>
     <row r="280" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F280" s="67"/>
+      <c r="F280" s="43"/>
     </row>
     <row r="281" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F281" s="67"/>
+      <c r="F281" s="43"/>
     </row>
     <row r="282" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F282" s="67"/>
+      <c r="F282" s="43"/>
     </row>
     <row r="283" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F283" s="67"/>
+      <c r="F283" s="43"/>
     </row>
     <row r="284" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F284" s="67"/>
+      <c r="F284" s="43"/>
     </row>
     <row r="285" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F285" s="67"/>
+      <c r="F285" s="43"/>
     </row>
     <row r="286" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F286" s="67"/>
+      <c r="F286" s="43"/>
     </row>
     <row r="287" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F287" s="67"/>
+      <c r="F287" s="43"/>
     </row>
     <row r="288" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F288" s="67"/>
+      <c r="F288" s="43"/>
     </row>
     <row r="289" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F289" s="67"/>
+      <c r="F289" s="43"/>
     </row>
     <row r="290" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F290" s="67"/>
+      <c r="F290" s="43"/>
     </row>
     <row r="291" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F291" s="67"/>
+      <c r="F291" s="43"/>
     </row>
     <row r="292" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F292" s="67"/>
+      <c r="F292" s="43"/>
     </row>
     <row r="293" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F293" s="67"/>
+      <c r="F293" s="43"/>
     </row>
     <row r="294" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F294" s="67"/>
+      <c r="F294" s="43"/>
     </row>
     <row r="295" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F295" s="67"/>
+      <c r="F295" s="43"/>
     </row>
     <row r="296" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F296" s="67"/>
+      <c r="F296" s="43"/>
     </row>
     <row r="297" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F297" s="67"/>
+      <c r="F297" s="43"/>
     </row>
     <row r="298" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F298" s="67"/>
+      <c r="F298" s="43"/>
     </row>
     <row r="299" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F299" s="67"/>
+      <c r="F299" s="43"/>
     </row>
     <row r="300" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F300" s="67"/>
+      <c r="F300" s="43"/>
     </row>
     <row r="301" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F301" s="67"/>
+      <c r="F301" s="43"/>
     </row>
     <row r="302" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F302" s="67"/>
+      <c r="F302" s="43"/>
     </row>
     <row r="303" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F303" s="67"/>
+      <c r="F303" s="43"/>
     </row>
     <row r="304" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F304" s="67"/>
+      <c r="F304" s="43"/>
     </row>
     <row r="305" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F305" s="67"/>
+      <c r="F305" s="43"/>
     </row>
     <row r="306" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F306" s="67"/>
+      <c r="F306" s="43"/>
     </row>
     <row r="307" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F307" s="67"/>
+      <c r="F307" s="43"/>
     </row>
     <row r="308" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F308" s="67"/>
+      <c r="F308" s="43"/>
     </row>
     <row r="309" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F309" s="67"/>
+      <c r="F309" s="43"/>
     </row>
     <row r="310" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F310" s="67"/>
+      <c r="F310" s="43"/>
     </row>
     <row r="311" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F311" s="67"/>
+      <c r="F311" s="43"/>
     </row>
     <row r="312" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F312" s="67"/>
+      <c r="F312" s="43"/>
     </row>
     <row r="313" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F313" s="67"/>
+      <c r="F313" s="43"/>
     </row>
     <row r="314" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F314" s="67"/>
+      <c r="F314" s="43"/>
     </row>
     <row r="315" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F315" s="67"/>
+      <c r="F315" s="43"/>
     </row>
     <row r="316" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F316" s="67"/>
+      <c r="F316" s="43"/>
     </row>
     <row r="317" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F317" s="67"/>
+      <c r="F317" s="43"/>
     </row>
     <row r="318" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F318" s="67"/>
+      <c r="F318" s="43"/>
     </row>
     <row r="319" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F319" s="67"/>
+      <c r="F319" s="43"/>
     </row>
     <row r="320" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F320" s="67"/>
+      <c r="F320" s="43"/>
     </row>
     <row r="321" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F321" s="67"/>
+      <c r="F321" s="43"/>
     </row>
     <row r="322" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F322" s="67"/>
+      <c r="F322" s="43"/>
     </row>
     <row r="323" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F323" s="67"/>
+      <c r="F323" s="43"/>
     </row>
     <row r="324" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F324" s="67"/>
+      <c r="F324" s="43"/>
     </row>
     <row r="325" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F325" s="67"/>
+      <c r="F325" s="43"/>
     </row>
     <row r="326" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F326" s="67"/>
+      <c r="F326" s="43"/>
     </row>
     <row r="327" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F327" s="67"/>
+      <c r="F327" s="43"/>
     </row>
     <row r="328" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F328" s="67"/>
+      <c r="F328" s="43"/>
     </row>
     <row r="329" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F329" s="67"/>
+      <c r="F329" s="43"/>
     </row>
     <row r="330" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F330" s="67"/>
+      <c r="F330" s="43"/>
     </row>
     <row r="331" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F331" s="67"/>
+      <c r="F331" s="43"/>
     </row>
     <row r="332" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F332" s="67"/>
+      <c r="F332" s="43"/>
     </row>
     <row r="333" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F333" s="67"/>
+      <c r="F333" s="43"/>
     </row>
     <row r="334" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F334" s="67"/>
+      <c r="F334" s="43"/>
     </row>
     <row r="335" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F335" s="67"/>
+      <c r="F335" s="43"/>
     </row>
     <row r="336" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F336" s="67"/>
+      <c r="F336" s="43"/>
     </row>
     <row r="337" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F337" s="67"/>
+      <c r="F337" s="43"/>
     </row>
     <row r="338" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F338" s="67"/>
+      <c r="F338" s="43"/>
     </row>
     <row r="339" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F339" s="67"/>
+      <c r="F339" s="43"/>
     </row>
     <row r="340" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F340" s="67"/>
+      <c r="F340" s="43"/>
     </row>
     <row r="341" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F341" s="67"/>
+      <c r="F341" s="43"/>
     </row>
     <row r="342" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F342" s="67"/>
+      <c r="F342" s="43"/>
     </row>
     <row r="343" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F343" s="67"/>
+      <c r="F343" s="43"/>
     </row>
     <row r="344" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F344" s="67"/>
+      <c r="F344" s="43"/>
     </row>
     <row r="345" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F345" s="67"/>
+      <c r="F345" s="43"/>
     </row>
     <row r="346" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F346" s="67"/>
+      <c r="F346" s="43"/>
     </row>
     <row r="347" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F347" s="67"/>
+      <c r="F347" s="43"/>
     </row>
     <row r="348" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F348" s="67"/>
+      <c r="F348" s="43"/>
     </row>
     <row r="349" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F349" s="67"/>
+      <c r="F349" s="43"/>
     </row>
     <row r="350" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F350" s="67"/>
+      <c r="F350" s="43"/>
     </row>
     <row r="351" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F351" s="67"/>
+      <c r="F351" s="43"/>
     </row>
     <row r="352" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F352" s="67"/>
+      <c r="F352" s="43"/>
     </row>
     <row r="353" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F353" s="67"/>
+      <c r="F353" s="43"/>
     </row>
     <row r="354" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F354" s="67"/>
+      <c r="F354" s="43"/>
     </row>
     <row r="355" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F355" s="67"/>
+      <c r="F355" s="43"/>
     </row>
     <row r="356" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F356" s="67"/>
+      <c r="F356" s="43"/>
     </row>
     <row r="357" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F357" s="67"/>
+      <c r="F357" s="43"/>
     </row>
     <row r="358" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F358" s="67"/>
+      <c r="F358" s="43"/>
     </row>
     <row r="359" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F359" s="67"/>
+      <c r="F359" s="43"/>
     </row>
     <row r="360" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F360" s="67"/>
+      <c r="F360" s="43"/>
     </row>
     <row r="361" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F361" s="67"/>
+      <c r="F361" s="43"/>
     </row>
     <row r="362" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F362" s="67"/>
+      <c r="F362" s="43"/>
     </row>
     <row r="363" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F363" s="67"/>
+      <c r="F363" s="43"/>
     </row>
     <row r="364" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F364" s="67"/>
+      <c r="F364" s="43"/>
     </row>
     <row r="365" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F365" s="67"/>
+      <c r="F365" s="43"/>
     </row>
     <row r="366" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F366" s="67"/>
+      <c r="F366" s="43"/>
     </row>
     <row r="367" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F367" s="67"/>
+      <c r="F367" s="43"/>
     </row>
     <row r="368" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F368" s="67"/>
+      <c r="F368" s="43"/>
     </row>
     <row r="369" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F369" s="67"/>
+      <c r="F369" s="43"/>
     </row>
     <row r="370" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F370" s="67"/>
+      <c r="F370" s="43"/>
     </row>
     <row r="371" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F371" s="67"/>
+      <c r="F371" s="43"/>
     </row>
     <row r="372" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F372" s="67"/>
+      <c r="F372" s="43"/>
     </row>
     <row r="373" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F373" s="67"/>
+      <c r="F373" s="43"/>
     </row>
     <row r="374" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F374" s="67"/>
+      <c r="F374" s="43"/>
     </row>
     <row r="375" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F375" s="67"/>
+      <c r="F375" s="43"/>
     </row>
     <row r="376" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F376" s="67"/>
+      <c r="F376" s="43"/>
     </row>
     <row r="377" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F377" s="67"/>
+      <c r="F377" s="43"/>
     </row>
     <row r="378" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F378" s="67"/>
+      <c r="F378" s="43"/>
     </row>
     <row r="379" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F379" s="67"/>
+      <c r="F379" s="43"/>
     </row>
     <row r="380" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F380" s="67"/>
+      <c r="F380" s="43"/>
     </row>
     <row r="381" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F381" s="67"/>
+      <c r="F381" s="43"/>
     </row>
     <row r="382" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F382" s="67"/>
+      <c r="F382" s="43"/>
     </row>
     <row r="383" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F383" s="67"/>
+      <c r="F383" s="43"/>
     </row>
     <row r="384" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F384" s="67"/>
+      <c r="F384" s="43"/>
     </row>
     <row r="385" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F385" s="67"/>
+      <c r="F385" s="43"/>
     </row>
     <row r="386" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F386" s="67"/>
+      <c r="F386" s="43"/>
     </row>
     <row r="387" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F387" s="67"/>
+      <c r="F387" s="43"/>
     </row>
     <row r="388" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F388" s="67"/>
+      <c r="F388" s="43"/>
     </row>
     <row r="389" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F389" s="67"/>
+      <c r="F389" s="43"/>
     </row>
     <row r="390" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F390" s="67"/>
+      <c r="F390" s="43"/>
     </row>
     <row r="391" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F391" s="67"/>
+      <c r="F391" s="43"/>
     </row>
     <row r="392" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F392" s="67"/>
+      <c r="F392" s="43"/>
     </row>
     <row r="393" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F393" s="67"/>
+      <c r="F393" s="43"/>
     </row>
     <row r="394" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F394" s="67"/>
+      <c r="F394" s="43"/>
     </row>
     <row r="395" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F395" s="67"/>
+      <c r="F395" s="43"/>
     </row>
     <row r="396" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F396" s="67"/>
+      <c r="F396" s="43"/>
     </row>
     <row r="397" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F397" s="67"/>
+      <c r="F397" s="43"/>
     </row>
     <row r="398" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F398" s="67"/>
+      <c r="F398" s="43"/>
     </row>
     <row r="399" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F399" s="67"/>
+      <c r="F399" s="43"/>
     </row>
     <row r="400" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F400" s="67"/>
+      <c r="F400" s="43"/>
     </row>
     <row r="401" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F401" s="67"/>
+      <c r="F401" s="43"/>
     </row>
     <row r="402" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F402" s="67"/>
+      <c r="F402" s="43"/>
     </row>
     <row r="403" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F403" s="67"/>
+      <c r="F403" s="43"/>
     </row>
     <row r="404" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F404" s="67"/>
+      <c r="F404" s="43"/>
     </row>
     <row r="405" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F405" s="67"/>
+      <c r="F405" s="43"/>
     </row>
     <row r="406" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F406" s="67"/>
+      <c r="F406" s="43"/>
     </row>
     <row r="407" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F407" s="67"/>
+      <c r="F407" s="43"/>
     </row>
     <row r="408" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F408" s="67"/>
+      <c r="F408" s="43"/>
     </row>
     <row r="409" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F409" s="67"/>
+      <c r="F409" s="43"/>
     </row>
     <row r="410" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F410" s="67"/>
+      <c r="F410" s="43"/>
     </row>
     <row r="411" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F411" s="67"/>
+      <c r="F411" s="43"/>
     </row>
     <row r="412" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F412" s="67"/>
+      <c r="F412" s="43"/>
     </row>
     <row r="413" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F413" s="67"/>
+      <c r="F413" s="43"/>
     </row>
     <row r="414" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F414" s="67"/>
+      <c r="F414" s="43"/>
     </row>
     <row r="415" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F415" s="67"/>
+      <c r="F415" s="43"/>
     </row>
     <row r="416" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F416" s="67"/>
+      <c r="F416" s="43"/>
     </row>
     <row r="417" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F417" s="67"/>
+      <c r="F417" s="43"/>
     </row>
     <row r="418" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F418" s="67"/>
+      <c r="F418" s="43"/>
     </row>
     <row r="419" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F419" s="67"/>
+      <c r="F419" s="43"/>
     </row>
     <row r="420" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F420" s="67"/>
+      <c r="F420" s="43"/>
     </row>
     <row r="421" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F421" s="67"/>
+      <c r="F421" s="43"/>
     </row>
     <row r="422" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F422" s="67"/>
+      <c r="F422" s="43"/>
     </row>
     <row r="423" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F423" s="67"/>
+      <c r="F423" s="43"/>
     </row>
     <row r="424" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F424" s="67"/>
+      <c r="F424" s="43"/>
     </row>
     <row r="425" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F425" s="67"/>
+      <c r="F425" s="43"/>
     </row>
     <row r="426" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F426" s="67"/>
+      <c r="F426" s="43"/>
     </row>
     <row r="427" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F427" s="67"/>
+      <c r="F427" s="43"/>
     </row>
     <row r="428" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F428" s="67"/>
+      <c r="F428" s="43"/>
     </row>
     <row r="429" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F429" s="67"/>
+      <c r="F429" s="43"/>
     </row>
     <row r="430" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F430" s="67"/>
+      <c r="F430" s="43"/>
     </row>
     <row r="431" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F431" s="67"/>
+      <c r="F431" s="43"/>
     </row>
     <row r="432" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F432" s="67"/>
+      <c r="F432" s="43"/>
     </row>
     <row r="433" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F433" s="67"/>
+      <c r="F433" s="43"/>
     </row>
     <row r="434" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F434" s="67"/>
+      <c r="F434" s="43"/>
     </row>
     <row r="435" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F435" s="67"/>
+      <c r="F435" s="43"/>
     </row>
     <row r="436" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F436" s="67"/>
+      <c r="F436" s="43"/>
     </row>
     <row r="437" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F437" s="67"/>
+      <c r="F437" s="43"/>
     </row>
     <row r="438" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F438" s="67"/>
+      <c r="F438" s="43"/>
     </row>
     <row r="439" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F439" s="67"/>
+      <c r="F439" s="43"/>
     </row>
     <row r="440" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F440" s="67"/>
+      <c r="F440" s="43"/>
     </row>
     <row r="441" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F441" s="67"/>
+      <c r="F441" s="43"/>
     </row>
     <row r="442" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F442" s="67"/>
+      <c r="F442" s="43"/>
     </row>
     <row r="443" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F443" s="67"/>
+      <c r="F443" s="43"/>
     </row>
     <row r="444" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F444" s="67"/>
+      <c r="F444" s="43"/>
     </row>
     <row r="445" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F445" s="67"/>
+      <c r="F445" s="43"/>
     </row>
     <row r="446" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F446" s="67"/>
+      <c r="F446" s="43"/>
     </row>
     <row r="447" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F447" s="67"/>
+      <c r="F447" s="43"/>
     </row>
     <row r="448" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F448" s="67"/>
+      <c r="F448" s="43"/>
     </row>
     <row r="449" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F449" s="67"/>
+      <c r="F449" s="43"/>
     </row>
     <row r="450" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F450" s="67"/>
+      <c r="F450" s="43"/>
     </row>
     <row r="451" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F451" s="67"/>
+      <c r="F451" s="43"/>
     </row>
     <row r="452" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F452" s="67"/>
+      <c r="F452" s="43"/>
     </row>
     <row r="453" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F453" s="67"/>
+      <c r="F453" s="43"/>
     </row>
     <row r="454" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F454" s="67"/>
+      <c r="F454" s="43"/>
     </row>
     <row r="455" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F455" s="67"/>
+      <c r="F455" s="43"/>
     </row>
     <row r="456" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F456" s="67"/>
+      <c r="F456" s="43"/>
     </row>
     <row r="457" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F457" s="67"/>
+      <c r="F457" s="43"/>
     </row>
     <row r="458" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F458" s="67"/>
+      <c r="F458" s="43"/>
     </row>
     <row r="459" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F459" s="67"/>
+      <c r="F459" s="43"/>
     </row>
     <row r="460" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F460" s="67"/>
+      <c r="F460" s="43"/>
     </row>
     <row r="461" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F461" s="67"/>
+      <c r="F461" s="43"/>
     </row>
     <row r="462" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F462" s="67"/>
+      <c r="F462" s="43"/>
     </row>
     <row r="463" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F463" s="67"/>
+      <c r="F463" s="43"/>
     </row>
     <row r="464" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F464" s="67"/>
+      <c r="F464" s="43"/>
     </row>
     <row r="465" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F465" s="67"/>
+      <c r="F465" s="43"/>
     </row>
     <row r="466" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F466" s="67"/>
+      <c r="F466" s="43"/>
     </row>
     <row r="467" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F467" s="67"/>
+      <c r="F467" s="43"/>
     </row>
     <row r="468" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F468" s="67"/>
+      <c r="F468" s="43"/>
     </row>
     <row r="469" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F469" s="67"/>
+      <c r="F469" s="43"/>
     </row>
     <row r="470" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F470" s="67"/>
+      <c r="F470" s="43"/>
     </row>
     <row r="471" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F471" s="67"/>
+      <c r="F471" s="43"/>
     </row>
     <row r="472" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F472" s="67"/>
+      <c r="F472" s="43"/>
     </row>
     <row r="473" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F473" s="67"/>
+      <c r="F473" s="43"/>
     </row>
     <row r="474" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F474" s="67"/>
+      <c r="F474" s="43"/>
     </row>
     <row r="475" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F475" s="67"/>
+      <c r="F475" s="43"/>
     </row>
     <row r="476" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F476" s="67"/>
+      <c r="F476" s="43"/>
     </row>
     <row r="477" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F477" s="67"/>
+      <c r="F477" s="43"/>
     </row>
     <row r="478" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F478" s="67"/>
+      <c r="F478" s="43"/>
     </row>
     <row r="479" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F479" s="67"/>
+      <c r="F479" s="43"/>
     </row>
     <row r="480" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F480" s="67"/>
+      <c r="F480" s="43"/>
     </row>
     <row r="481" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F481" s="67"/>
+      <c r="F481" s="43"/>
     </row>
     <row r="482" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F482" s="67"/>
+      <c r="F482" s="43"/>
     </row>
     <row r="483" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F483" s="67"/>
+      <c r="F483" s="43"/>
     </row>
     <row r="484" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F484" s="67"/>
+      <c r="F484" s="43"/>
     </row>
     <row r="485" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F485" s="67"/>
+      <c r="F485" s="43"/>
     </row>
     <row r="486" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F486" s="67"/>
+      <c r="F486" s="43"/>
     </row>
     <row r="487" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F487" s="67"/>
+      <c r="F487" s="43"/>
     </row>
     <row r="488" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F488" s="67"/>
+      <c r="F488" s="43"/>
     </row>
     <row r="489" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F489" s="67"/>
+      <c r="F489" s="43"/>
     </row>
     <row r="490" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F490" s="67"/>
+      <c r="F490" s="43"/>
     </row>
     <row r="491" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F491" s="67"/>
+      <c r="F491" s="43"/>
     </row>
     <row r="492" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F492" s="67"/>
+      <c r="F492" s="43"/>
     </row>
     <row r="493" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F493" s="67"/>
+      <c r="F493" s="43"/>
     </row>
     <row r="494" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F494" s="67"/>
+      <c r="F494" s="43"/>
     </row>
     <row r="495" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F495" s="67"/>
+      <c r="F495" s="43"/>
     </row>
     <row r="496" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F496" s="67"/>
+      <c r="F496" s="43"/>
     </row>
     <row r="497" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F497" s="67"/>
+      <c r="F497" s="43"/>
     </row>
     <row r="498" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F498" s="67"/>
+      <c r="F498" s="43"/>
     </row>
     <row r="499" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F499" s="67"/>
+      <c r="F499" s="43"/>
     </row>
     <row r="500" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F500" s="67"/>
+      <c r="F500" s="43"/>
     </row>
     <row r="501" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F501" s="67"/>
+      <c r="F501" s="43"/>
     </row>
     <row r="502" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F502" s="67"/>
+      <c r="F502" s="43"/>
     </row>
     <row r="503" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F503" s="67"/>
+      <c r="F503" s="43"/>
     </row>
     <row r="504" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F504" s="67"/>
+      <c r="F504" s="43"/>
     </row>
     <row r="505" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F505" s="67"/>
+      <c r="F505" s="43"/>
     </row>
     <row r="506" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F506" s="67"/>
+      <c r="F506" s="43"/>
     </row>
     <row r="507" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F507" s="67"/>
+      <c r="F507" s="43"/>
     </row>
     <row r="508" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F508" s="67"/>
+      <c r="F508" s="43"/>
     </row>
     <row r="509" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F509" s="67"/>
+      <c r="F509" s="43"/>
     </row>
     <row r="510" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F510" s="67"/>
+      <c r="F510" s="43"/>
     </row>
     <row r="511" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F511" s="67"/>
+      <c r="F511" s="43"/>
     </row>
     <row r="512" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F512" s="67"/>
+      <c r="F512" s="43"/>
     </row>
     <row r="513" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F513" s="67"/>
+      <c r="F513" s="43"/>
     </row>
     <row r="514" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F514" s="67"/>
+      <c r="F514" s="43"/>
     </row>
     <row r="515" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F515" s="67"/>
+      <c r="F515" s="43"/>
     </row>
     <row r="516" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F516" s="67"/>
+      <c r="F516" s="43"/>
     </row>
     <row r="517" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F517" s="67"/>
+      <c r="F517" s="43"/>
     </row>
     <row r="518" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F518" s="67"/>
+      <c r="F518" s="43"/>
     </row>
     <row r="519" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F519" s="67"/>
+      <c r="F519" s="43"/>
     </row>
     <row r="520" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F520" s="67"/>
+      <c r="F520" s="43"/>
     </row>
     <row r="521" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F521" s="67"/>
+      <c r="F521" s="43"/>
     </row>
     <row r="522" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F522" s="67"/>
+      <c r="F522" s="43"/>
     </row>
     <row r="523" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F523" s="67"/>
+      <c r="F523" s="43"/>
     </row>
     <row r="524" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F524" s="67"/>
+      <c r="F524" s="43"/>
     </row>
     <row r="525" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F525" s="67"/>
+      <c r="F525" s="43"/>
     </row>
     <row r="526" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F526" s="67"/>
+      <c r="F526" s="43"/>
     </row>
     <row r="527" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F527" s="67"/>
+      <c r="F527" s="43"/>
     </row>
     <row r="528" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F528" s="67"/>
+      <c r="F528" s="43"/>
     </row>
     <row r="529" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F529" s="67"/>
+      <c r="F529" s="43"/>
     </row>
     <row r="530" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F530" s="67"/>
+      <c r="F530" s="43"/>
     </row>
     <row r="531" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F531" s="67"/>
+      <c r="F531" s="43"/>
     </row>
     <row r="532" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F532" s="67"/>
+      <c r="F532" s="43"/>
     </row>
     <row r="533" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F533" s="67"/>
+      <c r="F533" s="43"/>
     </row>
     <row r="534" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F534" s="67"/>
+      <c r="F534" s="43"/>
     </row>
     <row r="535" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F535" s="67"/>
+      <c r="F535" s="43"/>
     </row>
     <row r="536" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F536" s="67"/>
+      <c r="F536" s="43"/>
     </row>
     <row r="537" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F537" s="67"/>
+      <c r="F537" s="43"/>
     </row>
     <row r="538" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F538" s="67"/>
+      <c r="F538" s="43"/>
     </row>
     <row r="539" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F539" s="67"/>
+      <c r="F539" s="43"/>
     </row>
     <row r="540" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F540" s="67"/>
+      <c r="F540" s="43"/>
     </row>
     <row r="541" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F541" s="67"/>
+      <c r="F541" s="43"/>
     </row>
     <row r="542" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F542" s="67"/>
+      <c r="F542" s="43"/>
     </row>
     <row r="543" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F543" s="67"/>
+      <c r="F543" s="43"/>
     </row>
     <row r="544" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F544" s="67"/>
+      <c r="F544" s="43"/>
     </row>
     <row r="545" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F545" s="67"/>
+      <c r="F545" s="43"/>
     </row>
     <row r="546" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F546" s="67"/>
+      <c r="F546" s="43"/>
     </row>
     <row r="547" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F547" s="67"/>
+      <c r="F547" s="43"/>
     </row>
     <row r="548" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F548" s="67"/>
+      <c r="F548" s="43"/>
     </row>
     <row r="549" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F549" s="67"/>
+      <c r="F549" s="43"/>
     </row>
     <row r="550" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F550" s="67"/>
+      <c r="F550" s="43"/>
     </row>
     <row r="551" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F551" s="67"/>
+      <c r="F551" s="43"/>
     </row>
     <row r="552" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F552" s="67"/>
+      <c r="F552" s="43"/>
     </row>
     <row r="553" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F553" s="67"/>
+      <c r="F553" s="43"/>
     </row>
     <row r="554" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F554" s="67"/>
+      <c r="F554" s="43"/>
     </row>
     <row r="555" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F555" s="67"/>
+      <c r="F555" s="43"/>
     </row>
     <row r="556" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F556" s="67"/>
+      <c r="F556" s="43"/>
     </row>
     <row r="557" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F557" s="67"/>
+      <c r="F557" s="43"/>
     </row>
     <row r="558" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F558" s="67"/>
+      <c r="F558" s="43"/>
     </row>
     <row r="559" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F559" s="67"/>
+      <c r="F559" s="43"/>
     </row>
     <row r="560" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F560" s="67"/>
+      <c r="F560" s="43"/>
     </row>
     <row r="561" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F561" s="67"/>
+      <c r="F561" s="43"/>
     </row>
     <row r="562" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F562" s="67"/>
+      <c r="F562" s="43"/>
     </row>
     <row r="563" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F563" s="67"/>
+      <c r="F563" s="43"/>
     </row>
     <row r="564" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F564" s="67"/>
+      <c r="F564" s="43"/>
     </row>
     <row r="565" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F565" s="67"/>
+      <c r="F565" s="43"/>
     </row>
     <row r="566" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F566" s="67"/>
+      <c r="F566" s="43"/>
     </row>
     <row r="567" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F567" s="67"/>
+      <c r="F567" s="43"/>
     </row>
     <row r="568" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F568" s="67"/>
+      <c r="F568" s="43"/>
     </row>
     <row r="569" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F569" s="67"/>
+      <c r="F569" s="43"/>
     </row>
     <row r="570" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F570" s="67"/>
+      <c r="F570" s="43"/>
     </row>
     <row r="571" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F571" s="67"/>
+      <c r="F571" s="43"/>
     </row>
     <row r="572" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F572" s="67"/>
+      <c r="F572" s="43"/>
     </row>
     <row r="573" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F573" s="67"/>
+      <c r="F573" s="43"/>
     </row>
     <row r="574" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F574" s="67"/>
+      <c r="F574" s="43"/>
     </row>
     <row r="575" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F575" s="67"/>
+      <c r="F575" s="43"/>
     </row>
     <row r="576" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F576" s="67"/>
+      <c r="F576" s="43"/>
     </row>
     <row r="577" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F577" s="67"/>
+      <c r="F577" s="43"/>
     </row>
     <row r="578" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F578" s="67"/>
+      <c r="F578" s="43"/>
     </row>
     <row r="579" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F579" s="67"/>
+      <c r="F579" s="43"/>
     </row>
     <row r="580" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F580" s="67"/>
+      <c r="F580" s="43"/>
     </row>
     <row r="581" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F581" s="67"/>
+      <c r="F581" s="43"/>
     </row>
     <row r="582" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F582" s="67"/>
+      <c r="F582" s="43"/>
     </row>
     <row r="583" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F583" s="67"/>
+      <c r="F583" s="43"/>
     </row>
     <row r="584" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F584" s="67"/>
+      <c r="F584" s="43"/>
     </row>
     <row r="585" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F585" s="67"/>
+      <c r="F585" s="43"/>
     </row>
     <row r="586" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F586" s="67"/>
+      <c r="F586" s="43"/>
     </row>
     <row r="587" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F587" s="67"/>
+      <c r="F587" s="43"/>
     </row>
     <row r="588" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F588" s="67"/>
+      <c r="F588" s="43"/>
     </row>
     <row r="589" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F589" s="67"/>
+      <c r="F589" s="43"/>
     </row>
     <row r="590" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F590" s="67"/>
+      <c r="F590" s="43"/>
     </row>
     <row r="591" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F591" s="67"/>
+      <c r="F591" s="43"/>
     </row>
     <row r="592" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F592" s="67"/>
+      <c r="F592" s="43"/>
     </row>
     <row r="593" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F593" s="67"/>
+      <c r="F593" s="43"/>
     </row>
     <row r="594" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F594" s="67"/>
+      <c r="F594" s="43"/>
     </row>
     <row r="595" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F595" s="67"/>
+      <c r="F595" s="43"/>
     </row>
     <row r="596" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F596" s="67"/>
+      <c r="F596" s="43"/>
     </row>
     <row r="597" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F597" s="67"/>
+      <c r="F597" s="43"/>
     </row>
     <row r="598" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F598" s="67"/>
+      <c r="F598" s="43"/>
     </row>
     <row r="599" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F599" s="67"/>
+      <c r="F599" s="43"/>
     </row>
     <row r="600" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F600" s="67"/>
+      <c r="F600" s="43"/>
     </row>
     <row r="601" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F601" s="67"/>
+      <c r="F601" s="43"/>
     </row>
     <row r="602" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F602" s="67"/>
+      <c r="F602" s="43"/>
     </row>
     <row r="603" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F603" s="67"/>
+      <c r="F603" s="43"/>
     </row>
     <row r="604" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F604" s="67"/>
+      <c r="F604" s="43"/>
     </row>
     <row r="605" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F605" s="67"/>
+      <c r="F605" s="43"/>
     </row>
     <row r="606" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F606" s="67"/>
+      <c r="F606" s="43"/>
     </row>
     <row r="607" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F607" s="67"/>
+      <c r="F607" s="43"/>
     </row>
     <row r="608" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F608" s="67"/>
+      <c r="F608" s="43"/>
     </row>
     <row r="609" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F609" s="67"/>
+      <c r="F609" s="43"/>
     </row>
     <row r="610" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F610" s="67"/>
+      <c r="F610" s="43"/>
     </row>
     <row r="611" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F611" s="67"/>
+      <c r="F611" s="43"/>
     </row>
     <row r="612" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F612" s="67"/>
+      <c r="F612" s="43"/>
     </row>
     <row r="613" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F613" s="67"/>
+      <c r="F613" s="43"/>
     </row>
     <row r="614" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F614" s="67"/>
+      <c r="F614" s="43"/>
     </row>
     <row r="615" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F615" s="67"/>
+      <c r="F615" s="43"/>
     </row>
     <row r="616" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F616" s="67"/>
+      <c r="F616" s="43"/>
     </row>
     <row r="617" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F617" s="67"/>
+      <c r="F617" s="43"/>
     </row>
     <row r="618" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F618" s="67"/>
+      <c r="F618" s="43"/>
     </row>
     <row r="619" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F619" s="67"/>
+      <c r="F619" s="43"/>
     </row>
     <row r="620" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F620" s="67"/>
+      <c r="F620" s="43"/>
     </row>
     <row r="621" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F621" s="67"/>
+      <c r="F621" s="43"/>
     </row>
     <row r="622" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F622" s="67"/>
+      <c r="F622" s="43"/>
     </row>
     <row r="623" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F623" s="67"/>
+      <c r="F623" s="43"/>
     </row>
     <row r="624" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F624" s="67"/>
+      <c r="F624" s="43"/>
     </row>
     <row r="625" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F625" s="67"/>
+      <c r="F625" s="43"/>
     </row>
     <row r="626" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F626" s="67"/>
+      <c r="F626" s="43"/>
     </row>
     <row r="627" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F627" s="67"/>
+      <c r="F627" s="43"/>
     </row>
     <row r="628" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F628" s="67"/>
+      <c r="F628" s="43"/>
     </row>
     <row r="629" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F629" s="67"/>
+      <c r="F629" s="43"/>
     </row>
     <row r="630" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F630" s="67"/>
+      <c r="F630" s="43"/>
     </row>
     <row r="631" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F631" s="67"/>
+      <c r="F631" s="43"/>
     </row>
     <row r="632" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F632" s="67"/>
+      <c r="F632" s="43"/>
     </row>
     <row r="633" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F633" s="67"/>
+      <c r="F633" s="43"/>
     </row>
     <row r="634" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F634" s="67"/>
+      <c r="F634" s="43"/>
     </row>
     <row r="635" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F635" s="67"/>
+      <c r="F635" s="43"/>
     </row>
     <row r="636" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F636" s="67"/>
+      <c r="F636" s="43"/>
     </row>
     <row r="637" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F637" s="67"/>
+      <c r="F637" s="43"/>
     </row>
     <row r="638" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F638" s="67"/>
+      <c r="F638" s="43"/>
     </row>
     <row r="639" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F639" s="67"/>
+      <c r="F639" s="43"/>
     </row>
     <row r="640" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F640" s="67"/>
+      <c r="F640" s="43"/>
     </row>
     <row r="641" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F641" s="67"/>
+      <c r="F641" s="43"/>
     </row>
     <row r="642" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F642" s="67"/>
+      <c r="F642" s="43"/>
     </row>
     <row r="643" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F643" s="67"/>
+      <c r="F643" s="43"/>
     </row>
     <row r="644" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F644" s="67"/>
+      <c r="F644" s="43"/>
     </row>
     <row r="645" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F645" s="67"/>
+      <c r="F645" s="43"/>
     </row>
     <row r="646" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F646" s="67"/>
+      <c r="F646" s="43"/>
     </row>
     <row r="647" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F647" s="67"/>
+      <c r="F647" s="43"/>
     </row>
     <row r="648" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F648" s="67"/>
+      <c r="F648" s="43"/>
     </row>
     <row r="649" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F649" s="67"/>
+      <c r="F649" s="43"/>
     </row>
     <row r="650" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F650" s="67"/>
+      <c r="F650" s="43"/>
     </row>
     <row r="651" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F651" s="67"/>
+      <c r="F651" s="43"/>
     </row>
     <row r="652" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F652" s="67"/>
+      <c r="F652" s="43"/>
     </row>
     <row r="653" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F653" s="67"/>
+      <c r="F653" s="43"/>
     </row>
     <row r="654" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F654" s="67"/>
+      <c r="F654" s="43"/>
     </row>
     <row r="655" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F655" s="67"/>
+      <c r="F655" s="43"/>
     </row>
     <row r="656" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F656" s="67"/>
+      <c r="F656" s="43"/>
     </row>
     <row r="657" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F657" s="67"/>
+      <c r="F657" s="43"/>
     </row>
     <row r="658" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F658" s="67"/>
+      <c r="F658" s="43"/>
     </row>
     <row r="659" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F659" s="67"/>
+      <c r="F659" s="43"/>
     </row>
     <row r="660" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F660" s="67"/>
+      <c r="F660" s="43"/>
     </row>
     <row r="661" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F661" s="67"/>
+      <c r="F661" s="43"/>
     </row>
     <row r="662" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F662" s="67"/>
+      <c r="F662" s="43"/>
     </row>
     <row r="663" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F663" s="67"/>
+      <c r="F663" s="43"/>
     </row>
     <row r="664" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F664" s="67"/>
+      <c r="F664" s="43"/>
     </row>
     <row r="665" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F665" s="67"/>
+      <c r="F665" s="43"/>
     </row>
     <row r="666" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F666" s="67"/>
+      <c r="F666" s="43"/>
     </row>
     <row r="667" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F667" s="67"/>
+      <c r="F667" s="43"/>
     </row>
     <row r="668" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F668" s="67"/>
+      <c r="F668" s="43"/>
     </row>
     <row r="669" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F669" s="67"/>
+      <c r="F669" s="43"/>
     </row>
     <row r="670" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F670" s="67"/>
+      <c r="F670" s="43"/>
     </row>
     <row r="671" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F671" s="67"/>
+      <c r="F671" s="43"/>
     </row>
     <row r="672" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F672" s="67"/>
+      <c r="F672" s="43"/>
     </row>
     <row r="673" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F673" s="67"/>
+      <c r="F673" s="43"/>
     </row>
     <row r="674" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F674" s="67"/>
+      <c r="F674" s="43"/>
     </row>
     <row r="675" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F675" s="67"/>
+      <c r="F675" s="43"/>
     </row>
     <row r="676" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F676" s="67"/>
+      <c r="F676" s="43"/>
     </row>
     <row r="677" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F677" s="67"/>
+      <c r="F677" s="43"/>
     </row>
     <row r="678" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F678" s="67"/>
+      <c r="F678" s="43"/>
     </row>
     <row r="679" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F679" s="67"/>
+      <c r="F679" s="43"/>
     </row>
     <row r="680" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F680" s="67"/>
+      <c r="F680" s="43"/>
     </row>
     <row r="681" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F681" s="67"/>
+      <c r="F681" s="43"/>
     </row>
     <row r="682" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F682" s="67"/>
+      <c r="F682" s="43"/>
     </row>
     <row r="683" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F683" s="67"/>
+      <c r="F683" s="43"/>
     </row>
     <row r="684" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F684" s="67"/>
+      <c r="F684" s="43"/>
     </row>
     <row r="685" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F685" s="67"/>
+      <c r="F685" s="43"/>
     </row>
     <row r="686" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F686" s="67"/>
+      <c r="F686" s="43"/>
     </row>
     <row r="687" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F687" s="67"/>
+      <c r="F687" s="43"/>
     </row>
     <row r="688" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F688" s="67"/>
+      <c r="F688" s="43"/>
     </row>
     <row r="689" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F689" s="67"/>
+      <c r="F689" s="43"/>
     </row>
     <row r="690" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F690" s="67"/>
+      <c r="F690" s="43"/>
     </row>
     <row r="691" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F691" s="67"/>
+      <c r="F691" s="43"/>
     </row>
     <row r="692" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F692" s="67"/>
+      <c r="F692" s="43"/>
     </row>
     <row r="693" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F693" s="67"/>
+      <c r="F693" s="43"/>
     </row>
     <row r="694" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F694" s="67"/>
+      <c r="F694" s="43"/>
     </row>
     <row r="695" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F695" s="67"/>
+      <c r="F695" s="43"/>
     </row>
     <row r="696" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F696" s="67"/>
+      <c r="F696" s="43"/>
     </row>
     <row r="697" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F697" s="67"/>
+      <c r="F697" s="43"/>
     </row>
     <row r="698" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F698" s="67"/>
+      <c r="F698" s="43"/>
     </row>
     <row r="699" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F699" s="67"/>
+      <c r="F699" s="43"/>
     </row>
     <row r="700" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F700" s="67"/>
+      <c r="F700" s="43"/>
     </row>
     <row r="701" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F701" s="67"/>
+      <c r="F701" s="43"/>
     </row>
     <row r="702" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F702" s="67"/>
+      <c r="F702" s="43"/>
     </row>
     <row r="703" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F703" s="67"/>
+      <c r="F703" s="43"/>
     </row>
     <row r="704" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F704" s="67"/>
+      <c r="F704" s="43"/>
     </row>
     <row r="705" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F705" s="67"/>
+      <c r="F705" s="43"/>
     </row>
     <row r="706" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F706" s="67"/>
+      <c r="F706" s="43"/>
     </row>
     <row r="707" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F707" s="67"/>
+      <c r="F707" s="43"/>
     </row>
     <row r="708" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F708" s="67"/>
+      <c r="F708" s="43"/>
     </row>
     <row r="709" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F709" s="67"/>
+      <c r="F709" s="43"/>
     </row>
     <row r="710" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F710" s="67"/>
+      <c r="F710" s="43"/>
     </row>
     <row r="711" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F711" s="67"/>
+      <c r="F711" s="43"/>
     </row>
     <row r="712" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F712" s="67"/>
+      <c r="F712" s="43"/>
     </row>
     <row r="713" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F713" s="67"/>
+      <c r="F713" s="43"/>
     </row>
     <row r="714" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F714" s="67"/>
+      <c r="F714" s="43"/>
     </row>
     <row r="715" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F715" s="67"/>
+      <c r="F715" s="43"/>
     </row>
     <row r="716" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F716" s="67"/>
+      <c r="F716" s="43"/>
     </row>
     <row r="717" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F717" s="67"/>
+      <c r="F717" s="43"/>
     </row>
     <row r="718" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F718" s="67"/>
+      <c r="F718" s="43"/>
     </row>
     <row r="719" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F719" s="67"/>
+      <c r="F719" s="43"/>
     </row>
     <row r="720" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F720" s="67"/>
+      <c r="F720" s="43"/>
     </row>
     <row r="721" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F721" s="67"/>
+      <c r="F721" s="43"/>
     </row>
     <row r="722" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F722" s="67"/>
+      <c r="F722" s="43"/>
     </row>
     <row r="723" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F723" s="67"/>
+      <c r="F723" s="43"/>
     </row>
     <row r="724" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F724" s="67"/>
+      <c r="F724" s="43"/>
     </row>
     <row r="725" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F725" s="67"/>
+      <c r="F725" s="43"/>
     </row>
     <row r="726" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F726" s="67"/>
+      <c r="F726" s="43"/>
     </row>
     <row r="727" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F727" s="67"/>
+      <c r="F727" s="43"/>
     </row>
     <row r="728" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F728" s="67"/>
+      <c r="F728" s="43"/>
     </row>
     <row r="729" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F729" s="67"/>
+      <c r="F729" s="43"/>
     </row>
     <row r="730" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F730" s="67"/>
+      <c r="F730" s="43"/>
     </row>
     <row r="731" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F731" s="67"/>
+      <c r="F731" s="43"/>
     </row>
     <row r="732" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F732" s="67"/>
+      <c r="F732" s="43"/>
     </row>
     <row r="733" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F733" s="67"/>
+      <c r="F733" s="43"/>
     </row>
     <row r="734" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F734" s="67"/>
+      <c r="F734" s="43"/>
     </row>
     <row r="735" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F735" s="67"/>
+      <c r="F735" s="43"/>
     </row>
     <row r="736" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F736" s="67"/>
+      <c r="F736" s="43"/>
     </row>
     <row r="737" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F737" s="67"/>
+      <c r="F737" s="43"/>
     </row>
     <row r="738" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F738" s="67"/>
+      <c r="F738" s="43"/>
     </row>
     <row r="739" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F739" s="67"/>
+      <c r="F739" s="43"/>
     </row>
     <row r="740" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F740" s="67"/>
+      <c r="F740" s="43"/>
     </row>
     <row r="741" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F741" s="67"/>
+      <c r="F741" s="43"/>
     </row>
     <row r="742" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F742" s="67"/>
+      <c r="F742" s="43"/>
     </row>
     <row r="743" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F743" s="67"/>
+      <c r="F743" s="43"/>
     </row>
     <row r="744" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F744" s="67"/>
+      <c r="F744" s="43"/>
     </row>
     <row r="745" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F745" s="67"/>
+      <c r="F745" s="43"/>
     </row>
     <row r="746" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F746" s="67"/>
+      <c r="F746" s="43"/>
     </row>
     <row r="747" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F747" s="67"/>
+      <c r="F747" s="43"/>
     </row>
     <row r="748" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F748" s="67"/>
+      <c r="F748" s="43"/>
     </row>
     <row r="749" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F749" s="67"/>
+      <c r="F749" s="43"/>
     </row>
     <row r="750" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F750" s="67"/>
+      <c r="F750" s="43"/>
     </row>
     <row r="751" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F751" s="67"/>
+      <c r="F751" s="43"/>
     </row>
     <row r="752" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F752" s="67"/>
+      <c r="F752" s="43"/>
     </row>
     <row r="753" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F753" s="67"/>
+      <c r="F753" s="43"/>
     </row>
     <row r="754" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F754" s="67"/>
+      <c r="F754" s="43"/>
     </row>
     <row r="755" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F755" s="67"/>
+      <c r="F755" s="43"/>
     </row>
     <row r="756" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F756" s="67"/>
+      <c r="F756" s="43"/>
     </row>
     <row r="757" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F757" s="67"/>
+      <c r="F757" s="43"/>
     </row>
     <row r="758" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F758" s="67"/>
+      <c r="F758" s="43"/>
     </row>
     <row r="759" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F759" s="67"/>
+      <c r="F759" s="43"/>
     </row>
     <row r="760" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F760" s="67"/>
+      <c r="F760" s="43"/>
     </row>
     <row r="761" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F761" s="67"/>
+      <c r="F761" s="43"/>
     </row>
     <row r="762" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F762" s="67"/>
+      <c r="F762" s="43"/>
     </row>
     <row r="763" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F763" s="67"/>
+      <c r="F763" s="43"/>
     </row>
     <row r="764" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F764" s="67"/>
+      <c r="F764" s="43"/>
     </row>
     <row r="765" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F765" s="67"/>
+      <c r="F765" s="43"/>
     </row>
     <row r="766" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F766" s="67"/>
+      <c r="F766" s="43"/>
     </row>
     <row r="767" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F767" s="67"/>
+      <c r="F767" s="43"/>
     </row>
     <row r="768" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F768" s="67"/>
+      <c r="F768" s="43"/>
     </row>
     <row r="769" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F769" s="67"/>
+      <c r="F769" s="43"/>
     </row>
     <row r="770" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F770" s="67"/>
+      <c r="F770" s="43"/>
     </row>
     <row r="771" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F771" s="67"/>
+      <c r="F771" s="43"/>
     </row>
     <row r="772" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F772" s="67"/>
+      <c r="F772" s="43"/>
     </row>
     <row r="773" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F773" s="67"/>
+      <c r="F773" s="43"/>
     </row>
     <row r="774" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F774" s="67"/>
+      <c r="F774" s="43"/>
     </row>
     <row r="775" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F775" s="67"/>
+      <c r="F775" s="43"/>
     </row>
     <row r="776" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F776" s="67"/>
+      <c r="F776" s="43"/>
     </row>
     <row r="777" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F777" s="67"/>
+      <c r="F777" s="43"/>
     </row>
     <row r="778" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F778" s="67"/>
+      <c r="F778" s="43"/>
     </row>
     <row r="779" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F779" s="67"/>
+      <c r="F779" s="43"/>
     </row>
     <row r="780" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F780" s="67"/>
+      <c r="F780" s="43"/>
     </row>
     <row r="781" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F781" s="67"/>
+      <c r="F781" s="43"/>
     </row>
     <row r="782" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F782" s="67"/>
+      <c r="F782" s="43"/>
     </row>
     <row r="783" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F783" s="67"/>
+      <c r="F783" s="43"/>
     </row>
     <row r="784" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F784" s="67"/>
+      <c r="F784" s="43"/>
     </row>
     <row r="785" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F785" s="67"/>
+      <c r="F785" s="43"/>
     </row>
     <row r="786" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F786" s="67"/>
+      <c r="F786" s="43"/>
     </row>
     <row r="787" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F787" s="67"/>
+      <c r="F787" s="43"/>
     </row>
     <row r="788" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F788" s="67"/>
+      <c r="F788" s="43"/>
     </row>
     <row r="789" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F789" s="67"/>
+      <c r="F789" s="43"/>
     </row>
     <row r="790" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F790" s="67"/>
+      <c r="F790" s="43"/>
     </row>
     <row r="791" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F791" s="67"/>
+      <c r="F791" s="43"/>
     </row>
     <row r="792" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F792" s="67"/>
+      <c r="F792" s="43"/>
     </row>
     <row r="793" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F793" s="67"/>
+      <c r="F793" s="43"/>
     </row>
     <row r="794" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F794" s="67"/>
+      <c r="F794" s="43"/>
     </row>
     <row r="795" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F795" s="67"/>
+      <c r="F795" s="43"/>
     </row>
     <row r="796" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F796" s="67"/>
+      <c r="F796" s="43"/>
     </row>
     <row r="797" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F797" s="67"/>
+      <c r="F797" s="43"/>
     </row>
     <row r="798" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F798" s="67"/>
+      <c r="F798" s="43"/>
     </row>
     <row r="799" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F799" s="67"/>
+      <c r="F799" s="43"/>
     </row>
     <row r="800" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F800" s="67"/>
+      <c r="F800" s="43"/>
     </row>
     <row r="801" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F801" s="67"/>
+      <c r="F801" s="43"/>
     </row>
     <row r="802" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F802" s="67"/>
+      <c r="F802" s="43"/>
     </row>
     <row r="803" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F803" s="67"/>
+      <c r="F803" s="43"/>
     </row>
     <row r="804" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F804" s="67"/>
+      <c r="F804" s="43"/>
     </row>
     <row r="805" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F805" s="67"/>
+      <c r="F805" s="43"/>
     </row>
     <row r="806" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F806" s="67"/>
+      <c r="F806" s="43"/>
     </row>
     <row r="807" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F807" s="67"/>
+      <c r="F807" s="43"/>
     </row>
     <row r="808" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F808" s="67"/>
+      <c r="F808" s="43"/>
     </row>
     <row r="809" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F809" s="67"/>
+      <c r="F809" s="43"/>
     </row>
     <row r="810" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F810" s="67"/>
+      <c r="F810" s="43"/>
     </row>
     <row r="811" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F811" s="67"/>
+      <c r="F811" s="43"/>
     </row>
     <row r="812" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F812" s="67"/>
+      <c r="F812" s="43"/>
     </row>
     <row r="813" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F813" s="67"/>
+      <c r="F813" s="43"/>
     </row>
     <row r="814" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F814" s="67"/>
+      <c r="F814" s="43"/>
     </row>
     <row r="815" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F815" s="67"/>
+      <c r="F815" s="43"/>
     </row>
     <row r="816" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F816" s="67"/>
+      <c r="F816" s="43"/>
     </row>
     <row r="817" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F817" s="67"/>
+      <c r="F817" s="43"/>
     </row>
     <row r="818" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F818" s="67"/>
+      <c r="F818" s="43"/>
     </row>
     <row r="819" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F819" s="67"/>
+      <c r="F819" s="43"/>
     </row>
     <row r="820" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F820" s="67"/>
+      <c r="F820" s="43"/>
     </row>
     <row r="821" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F821" s="67"/>
+      <c r="F821" s="43"/>
     </row>
     <row r="822" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F822" s="67"/>
+      <c r="F822" s="43"/>
     </row>
     <row r="823" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F823" s="67"/>
+      <c r="F823" s="43"/>
     </row>
     <row r="824" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F824" s="67"/>
+      <c r="F824" s="43"/>
     </row>
     <row r="825" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F825" s="67"/>
+      <c r="F825" s="43"/>
     </row>
     <row r="826" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F826" s="67"/>
+      <c r="F826" s="43"/>
     </row>
     <row r="827" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F827" s="67"/>
+      <c r="F827" s="43"/>
     </row>
     <row r="828" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F828" s="67"/>
+      <c r="F828" s="43"/>
     </row>
     <row r="829" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F829" s="67"/>
+      <c r="F829" s="43"/>
     </row>
     <row r="830" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F830" s="67"/>
+      <c r="F830" s="43"/>
     </row>
     <row r="831" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F831" s="67"/>
+      <c r="F831" s="43"/>
     </row>
     <row r="832" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F832" s="67"/>
+      <c r="F832" s="43"/>
     </row>
     <row r="833" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F833" s="67"/>
+      <c r="F833" s="43"/>
     </row>
     <row r="834" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F834" s="67"/>
+      <c r="F834" s="43"/>
     </row>
     <row r="835" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F835" s="67"/>
+      <c r="F835" s="43"/>
     </row>
     <row r="836" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F836" s="67"/>
+      <c r="F836" s="43"/>
     </row>
     <row r="837" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F837" s="67"/>
+      <c r="F837" s="43"/>
     </row>
     <row r="838" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F838" s="67"/>
+      <c r="F838" s="43"/>
     </row>
     <row r="839" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F839" s="67"/>
+      <c r="F839" s="43"/>
     </row>
     <row r="840" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F840" s="67"/>
+      <c r="F840" s="43"/>
     </row>
     <row r="841" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F841" s="67"/>
+      <c r="F841" s="43"/>
     </row>
     <row r="842" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F842" s="67"/>
+      <c r="F842" s="43"/>
     </row>
     <row r="843" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F843" s="67"/>
+      <c r="F843" s="43"/>
     </row>
     <row r="844" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F844" s="67"/>
+      <c r="F844" s="43"/>
     </row>
     <row r="845" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F845" s="67"/>
+      <c r="F845" s="43"/>
     </row>
     <row r="846" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F846" s="67"/>
+      <c r="F846" s="43"/>
     </row>
     <row r="847" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F847" s="67"/>
+      <c r="F847" s="43"/>
     </row>
     <row r="848" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F848" s="67"/>
+      <c r="F848" s="43"/>
     </row>
     <row r="849" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F849" s="67"/>
+      <c r="F849" s="43"/>
     </row>
     <row r="850" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F850" s="67"/>
+      <c r="F850" s="43"/>
     </row>
     <row r="851" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F851" s="67"/>
+      <c r="F851" s="43"/>
     </row>
     <row r="852" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F852" s="67"/>
+      <c r="F852" s="43"/>
     </row>
     <row r="853" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F853" s="67"/>
+      <c r="F853" s="43"/>
     </row>
     <row r="854" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F854" s="67"/>
+      <c r="F854" s="43"/>
     </row>
     <row r="855" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F855" s="67"/>
+      <c r="F855" s="43"/>
     </row>
     <row r="856" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F856" s="67"/>
+      <c r="F856" s="43"/>
     </row>
     <row r="857" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F857" s="67"/>
+      <c r="F857" s="43"/>
     </row>
     <row r="858" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F858" s="67"/>
+      <c r="F858" s="43"/>
     </row>
     <row r="859" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F859" s="67"/>
+      <c r="F859" s="43"/>
     </row>
     <row r="860" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F860" s="67"/>
+      <c r="F860" s="43"/>
     </row>
     <row r="861" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F861" s="67"/>
+      <c r="F861" s="43"/>
     </row>
     <row r="862" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F862" s="67"/>
+      <c r="F862" s="43"/>
     </row>
     <row r="863" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F863" s="67"/>
+      <c r="F863" s="43"/>
     </row>
     <row r="864" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F864" s="67"/>
+      <c r="F864" s="43"/>
     </row>
     <row r="865" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F865" s="67"/>
+      <c r="F865" s="43"/>
     </row>
     <row r="866" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F866" s="67"/>
+      <c r="F866" s="43"/>
     </row>
     <row r="867" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F867" s="67"/>
+      <c r="F867" s="43"/>
     </row>
     <row r="868" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F868" s="67"/>
+      <c r="F868" s="43"/>
     </row>
     <row r="869" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F869" s="67"/>
+      <c r="F869" s="43"/>
     </row>
     <row r="870" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F870" s="67"/>
+      <c r="F870" s="43"/>
     </row>
     <row r="871" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F871" s="67"/>
+      <c r="F871" s="43"/>
     </row>
     <row r="872" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F872" s="67"/>
+      <c r="F872" s="43"/>
     </row>
     <row r="873" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F873" s="67"/>
+      <c r="F873" s="43"/>
     </row>
     <row r="874" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F874" s="67"/>
+      <c r="F874" s="43"/>
     </row>
     <row r="875" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F875" s="67"/>
+      <c r="F875" s="43"/>
     </row>
     <row r="876" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F876" s="67"/>
+      <c r="F876" s="43"/>
     </row>
     <row r="877" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F877" s="67"/>
+      <c r="F877" s="43"/>
     </row>
     <row r="878" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F878" s="67"/>
+      <c r="F878" s="43"/>
     </row>
     <row r="879" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F879" s="67"/>
+      <c r="F879" s="43"/>
     </row>
     <row r="880" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F880" s="67"/>
+      <c r="F880" s="43"/>
     </row>
     <row r="881" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F881" s="67"/>
+      <c r="F881" s="43"/>
     </row>
     <row r="882" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F882" s="67"/>
+      <c r="F882" s="43"/>
     </row>
     <row r="883" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F883" s="67"/>
+      <c r="F883" s="43"/>
     </row>
     <row r="884" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F884" s="67"/>
+      <c r="F884" s="43"/>
     </row>
     <row r="885" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F885" s="67"/>
+      <c r="F885" s="43"/>
     </row>
     <row r="886" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F886" s="67"/>
+      <c r="F886" s="43"/>
     </row>
     <row r="887" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F887" s="67"/>
+      <c r="F887" s="43"/>
     </row>
     <row r="888" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F888" s="67"/>
+      <c r="F888" s="43"/>
     </row>
     <row r="889" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F889" s="67"/>
+      <c r="F889" s="43"/>
     </row>
     <row r="890" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F890" s="67"/>
+      <c r="F890" s="43"/>
     </row>
     <row r="891" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F891" s="67"/>
+      <c r="F891" s="43"/>
     </row>
     <row r="892" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F892" s="67"/>
+      <c r="F892" s="43"/>
     </row>
     <row r="893" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F893" s="67"/>
+      <c r="F893" s="43"/>
     </row>
     <row r="894" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F894" s="67"/>
+      <c r="F894" s="43"/>
     </row>
     <row r="895" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F895" s="67"/>
+      <c r="F895" s="43"/>
     </row>
     <row r="896" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F896" s="67"/>
+      <c r="F896" s="43"/>
     </row>
     <row r="897" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F897" s="67"/>
+      <c r="F897" s="43"/>
     </row>
     <row r="898" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F898" s="67"/>
+      <c r="F898" s="43"/>
     </row>
     <row r="899" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F899" s="67"/>
+      <c r="F899" s="43"/>
     </row>
     <row r="900" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F900" s="67"/>
+      <c r="F900" s="43"/>
     </row>
     <row r="901" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F901" s="67"/>
+      <c r="F901" s="43"/>
     </row>
     <row r="902" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F902" s="67"/>
+      <c r="F902" s="43"/>
     </row>
     <row r="903" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F903" s="67"/>
+      <c r="F903" s="43"/>
     </row>
     <row r="904" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F904" s="67"/>
+      <c r="F904" s="43"/>
     </row>
     <row r="905" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F905" s="67"/>
+      <c r="F905" s="43"/>
     </row>
     <row r="906" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F906" s="67"/>
+      <c r="F906" s="43"/>
     </row>
     <row r="907" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F907" s="67"/>
+      <c r="F907" s="43"/>
     </row>
     <row r="908" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F908" s="67"/>
+      <c r="F908" s="43"/>
     </row>
     <row r="909" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F909" s="67"/>
+      <c r="F909" s="43"/>
     </row>
     <row r="910" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F910" s="67"/>
+      <c r="F910" s="43"/>
     </row>
     <row r="911" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F911" s="67"/>
+      <c r="F911" s="43"/>
     </row>
     <row r="912" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F912" s="67"/>
+      <c r="F912" s="43"/>
     </row>
     <row r="913" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F913" s="67"/>
+      <c r="F913" s="43"/>
     </row>
     <row r="914" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F914" s="67"/>
+      <c r="F914" s="43"/>
     </row>
     <row r="915" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F915" s="67"/>
+      <c r="F915" s="43"/>
     </row>
     <row r="916" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F916" s="67"/>
+      <c r="F916" s="43"/>
     </row>
     <row r="917" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F917" s="67"/>
+      <c r="F917" s="43"/>
     </row>
     <row r="918" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F918" s="67"/>
+      <c r="F918" s="43"/>
     </row>
     <row r="919" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F919" s="67"/>
+      <c r="F919" s="43"/>
     </row>
     <row r="920" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F920" s="67"/>
+      <c r="F920" s="43"/>
     </row>
     <row r="921" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F921" s="67"/>
+      <c r="F921" s="43"/>
     </row>
     <row r="922" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F922" s="67"/>
+      <c r="F922" s="43"/>
     </row>
     <row r="923" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F923" s="67"/>
+      <c r="F923" s="43"/>
     </row>
     <row r="924" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F924" s="67"/>
+      <c r="F924" s="43"/>
     </row>
     <row r="925" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F925" s="67"/>
+      <c r="F925" s="43"/>
     </row>
     <row r="926" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F926" s="67"/>
+      <c r="F926" s="43"/>
     </row>
     <row r="927" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F927" s="67"/>
+      <c r="F927" s="43"/>
     </row>
     <row r="928" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F928" s="67"/>
+      <c r="F928" s="43"/>
     </row>
     <row r="929" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F929" s="67"/>
+      <c r="F929" s="43"/>
     </row>
     <row r="930" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F930" s="67"/>
+      <c r="F930" s="43"/>
     </row>
     <row r="931" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F931" s="67"/>
+      <c r="F931" s="43"/>
     </row>
     <row r="932" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F932" s="67"/>
+      <c r="F932" s="43"/>
     </row>
     <row r="933" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F933" s="67"/>
+      <c r="F933" s="43"/>
     </row>
     <row r="934" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F934" s="67"/>
+      <c r="F934" s="43"/>
     </row>
     <row r="935" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F935" s="67"/>
+      <c r="F935" s="43"/>
     </row>
     <row r="936" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F936" s="67"/>
+      <c r="F936" s="43"/>
     </row>
     <row r="937" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F937" s="67"/>
+      <c r="F937" s="43"/>
     </row>
     <row r="938" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F938" s="67"/>
+      <c r="F938" s="43"/>
     </row>
     <row r="939" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F939" s="67"/>
+      <c r="F939" s="43"/>
     </row>
     <row r="940" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F940" s="67"/>
+      <c r="F940" s="43"/>
     </row>
     <row r="941" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F941" s="67"/>
+      <c r="F941" s="43"/>
     </row>
     <row r="942" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F942" s="67"/>
+      <c r="F942" s="43"/>
     </row>
     <row r="943" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F943" s="67"/>
+      <c r="F943" s="43"/>
     </row>
     <row r="944" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F944" s="67"/>
+      <c r="F944" s="43"/>
     </row>
     <row r="945" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F945" s="67"/>
+      <c r="F945" s="43"/>
     </row>
     <row r="946" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F946" s="67"/>
+      <c r="F946" s="43"/>
     </row>
     <row r="947" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F947" s="67"/>
+      <c r="F947" s="43"/>
     </row>
     <row r="948" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F948" s="67"/>
+      <c r="F948" s="43"/>
     </row>
     <row r="949" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F949" s="67"/>
+      <c r="F949" s="43"/>
     </row>
     <row r="950" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F950" s="67"/>
+      <c r="F950" s="43"/>
     </row>
     <row r="951" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F951" s="67"/>
+      <c r="F951" s="43"/>
     </row>
     <row r="952" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F952" s="67"/>
+      <c r="F952" s="43"/>
     </row>
     <row r="953" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F953" s="67"/>
+      <c r="F953" s="43"/>
     </row>
     <row r="954" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F954" s="67"/>
+      <c r="F954" s="43"/>
     </row>
     <row r="955" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F955" s="67"/>
+      <c r="F955" s="43"/>
     </row>
     <row r="956" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F956" s="67"/>
+      <c r="F956" s="43"/>
     </row>
     <row r="957" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F957" s="67"/>
+      <c r="F957" s="43"/>
     </row>
     <row r="958" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F958" s="67"/>
+      <c r="F958" s="43"/>
     </row>
     <row r="959" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F959" s="67"/>
+      <c r="F959" s="43"/>
     </row>
     <row r="960" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F960" s="67"/>
+      <c r="F960" s="43"/>
     </row>
     <row r="961" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F961" s="67"/>
+      <c r="F961" s="43"/>
     </row>
     <row r="962" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F962" s="67"/>
+      <c r="F962" s="43"/>
     </row>
     <row r="963" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F963" s="67"/>
+      <c r="F963" s="43"/>
     </row>
     <row r="964" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F964" s="67"/>
+      <c r="F964" s="43"/>
     </row>
     <row r="965" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F965" s="67"/>
+      <c r="F965" s="43"/>
     </row>
     <row r="966" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F966" s="67"/>
+      <c r="F966" s="43"/>
     </row>
     <row r="967" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F967" s="67"/>
+      <c r="F967" s="43"/>
     </row>
     <row r="968" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F968" s="67"/>
+      <c r="F968" s="43"/>
     </row>
     <row r="969" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F969" s="67"/>
+      <c r="F969" s="43"/>
     </row>
     <row r="970" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F970" s="67"/>
+      <c r="F970" s="43"/>
     </row>
     <row r="971" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F971" s="67"/>
+      <c r="F971" s="43"/>
     </row>
     <row r="972" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F972" s="67"/>
-    </row>
-    <row r="973" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F973" s="67"/>
-    </row>
-    <row r="974" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F974" s="67"/>
-    </row>
-    <row r="975" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F975" s="67"/>
-    </row>
-    <row r="976" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F976" s="67"/>
-    </row>
-    <row r="977" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F977" s="67"/>
-    </row>
-    <row r="978" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F978" s="67"/>
+      <c r="F972" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="4">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A22:B25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A16:B19"/>
+    <mergeCell ref="F17:F19"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F27:F978 F17 F1:F7 F9:F15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F21:F972 F1:F7 F9:F14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4157,7 +4072,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4187,15 +4102,15 @@
         <v>8</v>
       </c>
       <c r="B2" s="15">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2" s="15">
-        <f>SUMIF(WP!C2:C21,"*Abdallah*",WP!D2:D21)</f>
-        <v>3</v>
+        <f>SUMIF(WP!C2:C15,"*Abdallah*",WP!D2:D15)</f>
+        <v>8</v>
       </c>
       <c r="D2" s="15">
-        <f>SUMIF(WP!C2:C21,"*Abdallah*",WP!E2:E21)</f>
-        <v>0</v>
+        <f>SUMIF(WP!C2:C15,"*Abdallah*",WP!E2:E15)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4206,12 +4121,12 @@
         <v>10</v>
       </c>
       <c r="C3" s="15">
-        <f>SUMIF(WP!C2:C21,"*Muhamed*",WP!D2:D21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Muhamed*",WP!D2:D15)</f>
+        <v>7</v>
       </c>
       <c r="D3" s="15">
-        <f>SUMIF(WP!C2:C21,"*Muhamed*",WP!E2:E21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Muhamed*",WP!E2:E15)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4222,12 +4137,12 @@
         <v>10</v>
       </c>
       <c r="C4" s="15">
-        <f>SUMIF(WP!C2:C21,"*Youstina*",WP!D2:D21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Youstina*",WP!D2:D15)</f>
+        <v>7</v>
       </c>
       <c r="D4" s="15">
-        <f>SUMIF(WP!C2:C21,"*Youstina*",WP!E2:E21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Youstina*",WP!E2:E15)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4238,12 +4153,12 @@
         <v>10</v>
       </c>
       <c r="C5" s="15">
-        <f>SUMIF(WP!C2:C21,"*Rana*",WP!D2:D21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Rana*",WP!D2:D15)</f>
+        <v>7</v>
       </c>
       <c r="D5" s="15">
-        <f>SUMIF(WP!C2:C21,"*Rana*",WP!E2:E21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Rana*",WP!E2:E15)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4254,12 +4169,12 @@
         <v>10</v>
       </c>
       <c r="C6" s="15">
-        <f>SUMIF(WP!C2:C21,"*Mariam*",WP!D2:D21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Mariam*",WP!D2:D15)</f>
+        <v>7</v>
       </c>
       <c r="D6" s="15">
-        <f>SUMIF(WP!C2:C21,"*Mariam*",WP!E2:E21)</f>
-        <v>2</v>
+        <f>SUMIF(WP!C2:C15,"*Mariam*",WP!E2:E15)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4268,15 +4183,15 @@
       </c>
       <c r="B7" s="16">
         <f>B2+B3+B4+B5+B6</f>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C7" s="16">
         <f>C2+C3+C4+C5+C6</f>
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D7" s="16">
         <f>D2+D3+D4+D5+D6</f>
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>